<commit_message>
Edit Alles verbeterd voor uitprinten
</commit_message>
<xml_diff>
--- a/Kt1/WP1.1/Moscow.xlsx
+++ b/Kt1/WP1.1/Moscow.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Naam functionaliteit</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Would Have</t>
   </si>
   <si>
-    <t>Inloggen</t>
-  </si>
-  <si>
     <t>Gebruikersnaam invoeren</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Melding onbekende username</t>
   </si>
   <si>
-    <t>Registreren</t>
-  </si>
-  <si>
     <t>Voornaam, Achternaam, Clientcode, geboortedatum kunnen invullen</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Melding fout wachtwoord administrator</t>
   </si>
   <si>
-    <t>Hoofdmenu</t>
-  </si>
-  <si>
     <t>Uitloggen</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>Melding zeker uitloggen ja/nee</t>
   </si>
   <si>
-    <t>Statistieken</t>
-  </si>
-  <si>
     <t>Scores bekijken van elke ingevulde lijst</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>Terug naar hoofdmenu knop</t>
   </si>
   <si>
-    <t>Vragenlijst</t>
-  </si>
-  <si>
     <t>Melding vraag niet ingevuld</t>
   </si>
   <si>
@@ -124,6 +109,21 @@
   </si>
   <si>
     <t>In procenten voortgang van de vragen</t>
+  </si>
+  <si>
+    <t>Functioneel</t>
+  </si>
+  <si>
+    <t>Grafische</t>
+  </si>
+  <si>
+    <t>Oranje/wit/blauw van huisstijl</t>
+  </si>
+  <si>
+    <t>Technisch</t>
+  </si>
+  <si>
+    <t>Windows phone ter beschikking</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -222,30 +222,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -254,10 +230,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
@@ -267,10 +239,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Controlecel" xfId="2" builtinId="23"/>
@@ -567,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B31:B32"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,223 +558,223 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.75" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="21">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:5">
       <c r="A2" s="8" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickTop="1">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" ht="30.75" thickTop="1">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="6" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickTop="1">
-      <c r="A13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A17" s="6" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="30.75" thickTop="1">
-      <c r="A19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A24" s="8" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="9"/>
@@ -806,86 +782,77 @@
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="1:5" ht="30.75" thickTop="1">
-      <c r="A25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+    <row r="25" spans="1:5">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="6" t="s">
-        <v>26</v>
+      <c r="A26" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A29" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A30" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickTop="1">
-      <c r="A31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="A28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="A32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>